<commit_message>
entered data until 22-06-16
</commit_message>
<xml_diff>
--- a/wordle.xlsx
+++ b/wordle.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julit\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julit\Documents\r_stuff\wordle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFE0E84-68F5-4334-8E6C-4292915C7120}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBCFF64-69F6-48F8-AC78-8764EBF4ADBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2825" uniqueCount="509">
   <si>
     <t>date</t>
   </si>
@@ -1312,6 +1312,246 @@
   </si>
   <si>
     <t>tamer</t>
+  </si>
+  <si>
+    <t>parch</t>
+  </si>
+  <si>
+    <t>scrap</t>
+  </si>
+  <si>
+    <t>veils</t>
+  </si>
+  <si>
+    <t>poney</t>
+  </si>
+  <si>
+    <t>money</t>
+  </si>
+  <si>
+    <t>token</t>
+  </si>
+  <si>
+    <t>honey</t>
+  </si>
+  <si>
+    <t>hinge</t>
+  </si>
+  <si>
+    <t>album</t>
+  </si>
+  <si>
+    <t>palms</t>
+  </si>
+  <si>
+    <t>almud</t>
+  </si>
+  <si>
+    <t>apply</t>
+  </si>
+  <si>
+    <t>spicy</t>
+  </si>
+  <si>
+    <t>bunch</t>
+  </si>
+  <si>
+    <t>gouch</t>
+  </si>
+  <si>
+    <t>vouch</t>
+  </si>
+  <si>
+    <t>polly</t>
+  </si>
+  <si>
+    <t>choco</t>
+  </si>
+  <si>
+    <t>asset</t>
+  </si>
+  <si>
+    <t>hated</t>
+  </si>
+  <si>
+    <t>vapes</t>
+  </si>
+  <si>
+    <t>ashen</t>
+  </si>
+  <si>
+    <t>stark</t>
+  </si>
+  <si>
+    <t>blart</t>
+  </si>
+  <si>
+    <t>tiara</t>
+  </si>
+  <si>
+    <t>crazy</t>
+  </si>
+  <si>
+    <t>alarm</t>
+  </si>
+  <si>
+    <t>crept</t>
+  </si>
+  <si>
+    <t>crest</t>
+  </si>
+  <si>
+    <t>maqui</t>
+  </si>
+  <si>
+    <t>bayou</t>
+  </si>
+  <si>
+    <t>baths</t>
+  </si>
+  <si>
+    <t>bacon</t>
+  </si>
+  <si>
+    <t>atoll</t>
+  </si>
+  <si>
+    <t>ramps</t>
+  </si>
+  <si>
+    <t>moral</t>
+  </si>
+  <si>
+    <t>mayor</t>
+  </si>
+  <si>
+    <t>creak</t>
+  </si>
+  <si>
+    <t>cream</t>
+  </si>
+  <si>
+    <t>showy</t>
+  </si>
+  <si>
+    <t>shows</t>
+  </si>
+  <si>
+    <t>shade</t>
+  </si>
+  <si>
+    <t>phase</t>
+  </si>
+  <si>
+    <t>shape</t>
+  </si>
+  <si>
+    <t>froth</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>petty</t>
+  </si>
+  <si>
+    <t>devon</t>
+  </si>
+  <si>
+    <t>deuce</t>
+  </si>
+  <si>
+    <t>gloom</t>
+  </si>
+  <si>
+    <t>whisms</t>
+  </si>
+  <si>
+    <t>mould</t>
+  </si>
+  <si>
+    <t>bloom</t>
+  </si>
+  <si>
+    <t>chomp</t>
+  </si>
+  <si>
+    <t>flood</t>
+  </si>
+  <si>
+    <t>solid</t>
+  </si>
+  <si>
+    <t>blood</t>
+  </si>
+  <si>
+    <t>trait</t>
+  </si>
+  <si>
+    <t>trans</t>
+  </si>
+  <si>
+    <t>prawn</t>
+  </si>
+  <si>
+    <t>track</t>
+  </si>
+  <si>
+    <t>girth</t>
+  </si>
+  <si>
+    <t>crown</t>
+  </si>
+  <si>
+    <t>slurp</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>goose</t>
+  </si>
+  <si>
+    <t>loose</t>
+  </si>
+  <si>
+    <t>teeny</t>
+  </si>
+  <si>
+    <t>piety</t>
+  </si>
+  <si>
+    <t>donor</t>
+  </si>
+  <si>
+    <t>horny</t>
+  </si>
+  <si>
+    <t>words</t>
+  </si>
+  <si>
+    <t>dormy</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>atone</t>
+  </si>
+  <si>
+    <t>primo</t>
+  </si>
+  <si>
+    <t>wrong</t>
+  </si>
+  <si>
+    <t>prior</t>
+  </si>
+  <si>
+    <t>apron</t>
+  </si>
+  <si>
+    <t>afros</t>
   </si>
 </sst>
 </file>
@@ -1636,11 +1876,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E766"/>
+  <dimension ref="A1:E941"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A750" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C766" sqref="C766"/>
+      <pane ySplit="1" topLeftCell="A924" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A942" sqref="A942"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14657,6 +14897,2993 @@
       <c r="A766" s="1">
         <v>44702</v>
       </c>
+      <c r="B766" t="s">
+        <v>430</v>
+      </c>
+      <c r="C766" t="s">
+        <v>8</v>
+      </c>
+      <c r="D766">
+        <v>1</v>
+      </c>
+      <c r="E766" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="767" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A767" s="1">
+        <v>44702</v>
+      </c>
+      <c r="B767" t="s">
+        <v>430</v>
+      </c>
+      <c r="C767" t="s">
+        <v>429</v>
+      </c>
+      <c r="D767">
+        <v>2</v>
+      </c>
+      <c r="E767" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="768" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A768" s="1">
+        <v>44702</v>
+      </c>
+      <c r="B768" t="s">
+        <v>430</v>
+      </c>
+      <c r="C768" t="s">
+        <v>430</v>
+      </c>
+      <c r="D768">
+        <v>3</v>
+      </c>
+      <c r="E768" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="769" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A769" s="1">
+        <v>44703</v>
+      </c>
+      <c r="B769" t="s">
+        <v>433</v>
+      </c>
+      <c r="C769" t="s">
+        <v>8</v>
+      </c>
+      <c r="D769">
+        <v>1</v>
+      </c>
+      <c r="E769" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="770" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A770" s="1">
+        <v>44703</v>
+      </c>
+      <c r="B770" t="s">
+        <v>433</v>
+      </c>
+      <c r="C770" t="s">
+        <v>431</v>
+      </c>
+      <c r="D770">
+        <v>2</v>
+      </c>
+      <c r="E770" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="771" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A771" s="1">
+        <v>44703</v>
+      </c>
+      <c r="B771" t="s">
+        <v>433</v>
+      </c>
+      <c r="C771" t="s">
+        <v>432</v>
+      </c>
+      <c r="D771">
+        <v>3</v>
+      </c>
+      <c r="E771" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="772" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A772" s="1">
+        <v>44703</v>
+      </c>
+      <c r="B772" t="s">
+        <v>433</v>
+      </c>
+      <c r="C772" t="s">
+        <v>433</v>
+      </c>
+      <c r="D772">
+        <v>4</v>
+      </c>
+      <c r="E772" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="773" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A773" s="1">
+        <v>44703</v>
+      </c>
+      <c r="B773" t="s">
+        <v>433</v>
+      </c>
+      <c r="C773" t="s">
+        <v>13</v>
+      </c>
+      <c r="D773">
+        <v>1</v>
+      </c>
+      <c r="E773" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="774" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A774" s="1">
+        <v>44703</v>
+      </c>
+      <c r="B774" t="s">
+        <v>433</v>
+      </c>
+      <c r="C774" t="s">
+        <v>62</v>
+      </c>
+      <c r="D774">
+        <v>2</v>
+      </c>
+      <c r="E774" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="775" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A775" s="1">
+        <v>44703</v>
+      </c>
+      <c r="B775" t="s">
+        <v>433</v>
+      </c>
+      <c r="C775" t="s">
+        <v>434</v>
+      </c>
+      <c r="D775">
+        <v>3</v>
+      </c>
+      <c r="E775" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="776" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A776" s="1">
+        <v>44703</v>
+      </c>
+      <c r="B776" t="s">
+        <v>433</v>
+      </c>
+      <c r="C776" t="s">
+        <v>435</v>
+      </c>
+      <c r="D776">
+        <v>4</v>
+      </c>
+      <c r="E776" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="777" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A777" s="1">
+        <v>44703</v>
+      </c>
+      <c r="B777" t="s">
+        <v>433</v>
+      </c>
+      <c r="C777" t="s">
+        <v>433</v>
+      </c>
+      <c r="D777">
+        <v>5</v>
+      </c>
+      <c r="E777" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="778" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A778" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B778" t="s">
+        <v>436</v>
+      </c>
+      <c r="C778" t="s">
+        <v>8</v>
+      </c>
+      <c r="D778">
+        <v>1</v>
+      </c>
+      <c r="E778" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="779" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A779" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B779" t="s">
+        <v>436</v>
+      </c>
+      <c r="C779" t="s">
+        <v>152</v>
+      </c>
+      <c r="D779">
+        <v>2</v>
+      </c>
+      <c r="E779" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="780" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A780" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B780" t="s">
+        <v>436</v>
+      </c>
+      <c r="C780" t="s">
+        <v>436</v>
+      </c>
+      <c r="D780">
+        <v>3</v>
+      </c>
+      <c r="E780" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="781" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A781" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B781" t="s">
+        <v>436</v>
+      </c>
+      <c r="C781" t="s">
+        <v>13</v>
+      </c>
+      <c r="D781">
+        <v>1</v>
+      </c>
+      <c r="E781" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="782" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A782" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B782" t="s">
+        <v>436</v>
+      </c>
+      <c r="C782" t="s">
+        <v>62</v>
+      </c>
+      <c r="D782">
+        <v>2</v>
+      </c>
+      <c r="E782" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="783" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A783" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B783" t="s">
+        <v>436</v>
+      </c>
+      <c r="C783" t="s">
+        <v>264</v>
+      </c>
+      <c r="D783">
+        <v>3</v>
+      </c>
+      <c r="E783" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="784" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A784" s="1">
+        <v>44704</v>
+      </c>
+      <c r="B784" t="s">
+        <v>436</v>
+      </c>
+      <c r="C784" t="s">
+        <v>436</v>
+      </c>
+      <c r="D784">
+        <v>4</v>
+      </c>
+      <c r="E784" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="785" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A785" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B785" t="s">
+        <v>437</v>
+      </c>
+      <c r="C785" t="s">
+        <v>8</v>
+      </c>
+      <c r="D785">
+        <v>1</v>
+      </c>
+      <c r="E785" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="786" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A786" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B786" t="s">
+        <v>437</v>
+      </c>
+      <c r="C786" t="s">
+        <v>438</v>
+      </c>
+      <c r="D786">
+        <v>2</v>
+      </c>
+      <c r="E786" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="787" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A787" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B787" t="s">
+        <v>437</v>
+      </c>
+      <c r="C787" t="s">
+        <v>439</v>
+      </c>
+      <c r="D787">
+        <v>3</v>
+      </c>
+      <c r="E787" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="788" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A788" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B788" t="s">
+        <v>437</v>
+      </c>
+      <c r="C788" t="s">
+        <v>437</v>
+      </c>
+      <c r="D788">
+        <v>4</v>
+      </c>
+      <c r="E788" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="789" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A789" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B789" t="s">
+        <v>437</v>
+      </c>
+      <c r="C789" t="s">
+        <v>13</v>
+      </c>
+      <c r="D789">
+        <v>1</v>
+      </c>
+      <c r="E789" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="790" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A790" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B790" t="s">
+        <v>437</v>
+      </c>
+      <c r="C790" t="s">
+        <v>29</v>
+      </c>
+      <c r="D790">
+        <v>2</v>
+      </c>
+      <c r="E790" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="791" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A791" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B791" t="s">
+        <v>437</v>
+      </c>
+      <c r="C791" t="s">
+        <v>440</v>
+      </c>
+      <c r="D791">
+        <v>3</v>
+      </c>
+      <c r="E791" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="792" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A792" s="1">
+        <v>44705</v>
+      </c>
+      <c r="B792" t="s">
+        <v>437</v>
+      </c>
+      <c r="C792" t="s">
+        <v>437</v>
+      </c>
+      <c r="D792">
+        <v>4</v>
+      </c>
+      <c r="E792" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="793" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A793" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B793" t="s">
+        <v>444</v>
+      </c>
+      <c r="C793" t="s">
+        <v>8</v>
+      </c>
+      <c r="D793">
+        <v>1</v>
+      </c>
+      <c r="E793" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="794" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A794" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B794" t="s">
+        <v>444</v>
+      </c>
+      <c r="C794" t="s">
+        <v>441</v>
+      </c>
+      <c r="D794">
+        <v>2</v>
+      </c>
+      <c r="E794" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="795" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A795" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B795" t="s">
+        <v>444</v>
+      </c>
+      <c r="C795" t="s">
+        <v>442</v>
+      </c>
+      <c r="D795">
+        <v>3</v>
+      </c>
+      <c r="E795" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="796" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A796" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B796" t="s">
+        <v>444</v>
+      </c>
+      <c r="C796" t="s">
+        <v>211</v>
+      </c>
+      <c r="D796">
+        <v>4</v>
+      </c>
+      <c r="E796" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="797" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A797" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B797" t="s">
+        <v>444</v>
+      </c>
+      <c r="C797" t="s">
+        <v>443</v>
+      </c>
+      <c r="D797">
+        <v>5</v>
+      </c>
+      <c r="E797" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="798" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A798" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B798" t="s">
+        <v>444</v>
+      </c>
+      <c r="C798" t="s">
+        <v>444</v>
+      </c>
+      <c r="D798">
+        <v>6</v>
+      </c>
+      <c r="E798" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="799" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A799" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B799" t="s">
+        <v>444</v>
+      </c>
+      <c r="C799" t="s">
+        <v>13</v>
+      </c>
+      <c r="D799">
+        <v>1</v>
+      </c>
+      <c r="E799" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="800" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A800" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B800" t="s">
+        <v>444</v>
+      </c>
+      <c r="C800" t="s">
+        <v>29</v>
+      </c>
+      <c r="D800">
+        <v>2</v>
+      </c>
+      <c r="E800" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="801" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A801" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B801" t="s">
+        <v>444</v>
+      </c>
+      <c r="C801" t="s">
+        <v>445</v>
+      </c>
+      <c r="D801">
+        <v>3</v>
+      </c>
+      <c r="E801" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="802" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A802" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B802" t="s">
+        <v>444</v>
+      </c>
+      <c r="C802" t="s">
+        <v>446</v>
+      </c>
+      <c r="D802">
+        <v>4</v>
+      </c>
+      <c r="E802" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="803" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A803" s="1">
+        <v>44706</v>
+      </c>
+      <c r="B803" t="s">
+        <v>444</v>
+      </c>
+      <c r="C803" t="s">
+        <v>444</v>
+      </c>
+      <c r="D803">
+        <v>5</v>
+      </c>
+      <c r="E803" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="804" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A804" s="1">
+        <v>44707</v>
+      </c>
+      <c r="B804" t="s">
+        <v>447</v>
+      </c>
+      <c r="C804" t="s">
+        <v>8</v>
+      </c>
+      <c r="D804">
+        <v>1</v>
+      </c>
+      <c r="E804" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="805" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A805" s="1">
+        <v>44707</v>
+      </c>
+      <c r="B805" t="s">
+        <v>447</v>
+      </c>
+      <c r="C805" t="s">
+        <v>448</v>
+      </c>
+      <c r="D805">
+        <v>2</v>
+      </c>
+      <c r="E805" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="806" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A806" s="1">
+        <v>44707</v>
+      </c>
+      <c r="B806" t="s">
+        <v>447</v>
+      </c>
+      <c r="C806" t="s">
+        <v>447</v>
+      </c>
+      <c r="D806">
+        <v>3</v>
+      </c>
+      <c r="E806" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="807" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A807" s="1">
+        <v>44707</v>
+      </c>
+      <c r="B807" t="s">
+        <v>447</v>
+      </c>
+      <c r="C807" t="s">
+        <v>13</v>
+      </c>
+      <c r="D807">
+        <v>1</v>
+      </c>
+      <c r="E807" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="808" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A808" s="1">
+        <v>44707</v>
+      </c>
+      <c r="B808" t="s">
+        <v>447</v>
+      </c>
+      <c r="C808" t="s">
+        <v>449</v>
+      </c>
+      <c r="D808">
+        <v>2</v>
+      </c>
+      <c r="E808" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="809" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A809" s="1">
+        <v>44707</v>
+      </c>
+      <c r="B809" t="s">
+        <v>447</v>
+      </c>
+      <c r="C809" t="s">
+        <v>450</v>
+      </c>
+      <c r="D809">
+        <v>3</v>
+      </c>
+      <c r="E809" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="810" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A810" s="1">
+        <v>44707</v>
+      </c>
+      <c r="B810" t="s">
+        <v>447</v>
+      </c>
+      <c r="C810" t="s">
+        <v>447</v>
+      </c>
+      <c r="D810">
+        <v>4</v>
+      </c>
+      <c r="E810" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="811" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A811" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B811" t="s">
+        <v>453</v>
+      </c>
+      <c r="C811" t="s">
+        <v>8</v>
+      </c>
+      <c r="D811">
+        <v>1</v>
+      </c>
+      <c r="E811" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="812" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A812" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B812" t="s">
+        <v>453</v>
+      </c>
+      <c r="C812" t="s">
+        <v>451</v>
+      </c>
+      <c r="D812">
+        <v>2</v>
+      </c>
+      <c r="E812" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="813" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A813" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B813" t="s">
+        <v>453</v>
+      </c>
+      <c r="C813" t="s">
+        <v>452</v>
+      </c>
+      <c r="D813">
+        <v>3</v>
+      </c>
+      <c r="E813" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="814" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A814" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B814" t="s">
+        <v>453</v>
+      </c>
+      <c r="C814" t="s">
+        <v>453</v>
+      </c>
+      <c r="D814">
+        <v>4</v>
+      </c>
+      <c r="E814" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="815" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A815" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B815" t="s">
+        <v>453</v>
+      </c>
+      <c r="C815" t="s">
+        <v>13</v>
+      </c>
+      <c r="D815">
+        <v>1</v>
+      </c>
+      <c r="E815" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="816" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A816" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B816" t="s">
+        <v>453</v>
+      </c>
+      <c r="C816" t="s">
+        <v>454</v>
+      </c>
+      <c r="D816">
+        <v>2</v>
+      </c>
+      <c r="E816" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="817" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A817" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B817" t="s">
+        <v>453</v>
+      </c>
+      <c r="C817" t="s">
+        <v>95</v>
+      </c>
+      <c r="D817">
+        <v>3</v>
+      </c>
+      <c r="E817" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="818" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A818" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B818" t="s">
+        <v>453</v>
+      </c>
+      <c r="C818" t="s">
+        <v>455</v>
+      </c>
+      <c r="D818">
+        <v>4</v>
+      </c>
+      <c r="E818" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="819" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A819" s="1">
+        <v>44708</v>
+      </c>
+      <c r="B819" t="s">
+        <v>453</v>
+      </c>
+      <c r="C819" t="s">
+        <v>453</v>
+      </c>
+      <c r="D819">
+        <v>5</v>
+      </c>
+      <c r="E819" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="820" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A820" s="1">
+        <v>44709</v>
+      </c>
+      <c r="B820" t="s">
+        <v>456</v>
+      </c>
+      <c r="C820" t="s">
+        <v>8</v>
+      </c>
+      <c r="D820">
+        <v>1</v>
+      </c>
+      <c r="E820" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="821" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A821" s="1">
+        <v>44709</v>
+      </c>
+      <c r="B821" t="s">
+        <v>456</v>
+      </c>
+      <c r="C821" t="s">
+        <v>457</v>
+      </c>
+      <c r="D821">
+        <v>2</v>
+      </c>
+      <c r="E821" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="822" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A822" s="1">
+        <v>44709</v>
+      </c>
+      <c r="B822" t="s">
+        <v>456</v>
+      </c>
+      <c r="C822" t="s">
+        <v>456</v>
+      </c>
+      <c r="D822">
+        <v>3</v>
+      </c>
+      <c r="E822" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="823" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A823" s="1">
+        <v>44710</v>
+      </c>
+      <c r="B823" t="s">
+        <v>459</v>
+      </c>
+      <c r="C823" t="s">
+        <v>8</v>
+      </c>
+      <c r="D823">
+        <v>1</v>
+      </c>
+      <c r="E823" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="824" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A824" s="1">
+        <v>44710</v>
+      </c>
+      <c r="B824" t="s">
+        <v>459</v>
+      </c>
+      <c r="C824" t="s">
+        <v>336</v>
+      </c>
+      <c r="D824">
+        <v>2</v>
+      </c>
+      <c r="E824" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="825" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A825" s="1">
+        <v>44710</v>
+      </c>
+      <c r="B825" t="s">
+        <v>459</v>
+      </c>
+      <c r="C825" t="s">
+        <v>332</v>
+      </c>
+      <c r="D825">
+        <v>3</v>
+      </c>
+      <c r="E825" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="826" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A826" s="1">
+        <v>44710</v>
+      </c>
+      <c r="B826" t="s">
+        <v>459</v>
+      </c>
+      <c r="C826" t="s">
+        <v>458</v>
+      </c>
+      <c r="D826">
+        <v>4</v>
+      </c>
+      <c r="E826" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="827" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A827" s="1">
+        <v>44710</v>
+      </c>
+      <c r="B827" t="s">
+        <v>459</v>
+      </c>
+      <c r="C827" t="s">
+        <v>459</v>
+      </c>
+      <c r="D827">
+        <v>5</v>
+      </c>
+      <c r="E827" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="828" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A828" s="1">
+        <v>44710</v>
+      </c>
+      <c r="B828" t="s">
+        <v>459</v>
+      </c>
+      <c r="C828" t="s">
+        <v>13</v>
+      </c>
+      <c r="D828">
+        <v>1</v>
+      </c>
+      <c r="E828" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="829" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A829" s="1">
+        <v>44710</v>
+      </c>
+      <c r="B829" t="s">
+        <v>459</v>
+      </c>
+      <c r="C829" t="s">
+        <v>460</v>
+      </c>
+      <c r="D829">
+        <v>2</v>
+      </c>
+      <c r="E829" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="830" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A830" s="1">
+        <v>44710</v>
+      </c>
+      <c r="B830" t="s">
+        <v>459</v>
+      </c>
+      <c r="C830" t="s">
+        <v>461</v>
+      </c>
+      <c r="D830">
+        <v>3</v>
+      </c>
+      <c r="E830" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="831" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A831" s="1">
+        <v>44710</v>
+      </c>
+      <c r="B831" t="s">
+        <v>459</v>
+      </c>
+      <c r="C831" t="s">
+        <v>459</v>
+      </c>
+      <c r="D831">
+        <v>4</v>
+      </c>
+      <c r="E831" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="832" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A832" s="1">
+        <v>44711</v>
+      </c>
+      <c r="B832" t="s">
+        <v>462</v>
+      </c>
+      <c r="C832" t="s">
+        <v>8</v>
+      </c>
+      <c r="D832">
+        <v>1</v>
+      </c>
+      <c r="E832" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="833" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A833" s="1">
+        <v>44711</v>
+      </c>
+      <c r="B833" t="s">
+        <v>462</v>
+      </c>
+      <c r="C833" t="s">
+        <v>226</v>
+      </c>
+      <c r="D833">
+        <v>2</v>
+      </c>
+      <c r="E833" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="834" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A834" s="1">
+        <v>44711</v>
+      </c>
+      <c r="B834" t="s">
+        <v>462</v>
+      </c>
+      <c r="C834" t="s">
+        <v>244</v>
+      </c>
+      <c r="D834">
+        <v>3</v>
+      </c>
+      <c r="E834" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="835" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A835" s="1">
+        <v>44711</v>
+      </c>
+      <c r="B835" t="s">
+        <v>462</v>
+      </c>
+      <c r="C835" t="s">
+        <v>462</v>
+      </c>
+      <c r="D835">
+        <v>4</v>
+      </c>
+      <c r="E835" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="836" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A836" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B836" t="s">
+        <v>349</v>
+      </c>
+      <c r="C836" t="s">
+        <v>8</v>
+      </c>
+      <c r="D836">
+        <v>1</v>
+      </c>
+      <c r="E836" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="837" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A837" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B837" t="s">
+        <v>349</v>
+      </c>
+      <c r="C837" t="s">
+        <v>463</v>
+      </c>
+      <c r="D837">
+        <v>2</v>
+      </c>
+      <c r="E837" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="838" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A838" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B838" t="s">
+        <v>349</v>
+      </c>
+      <c r="C838" t="s">
+        <v>349</v>
+      </c>
+      <c r="D838">
+        <v>3</v>
+      </c>
+      <c r="E838" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="839" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A839" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B839" t="s">
+        <v>349</v>
+      </c>
+      <c r="C839" t="s">
+        <v>13</v>
+      </c>
+      <c r="D839">
+        <v>1</v>
+      </c>
+      <c r="E839" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="840" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A840" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B840" t="s">
+        <v>349</v>
+      </c>
+      <c r="C840" t="s">
+        <v>464</v>
+      </c>
+      <c r="D840">
+        <v>2</v>
+      </c>
+      <c r="E840" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="841" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A841" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B841" t="s">
+        <v>349</v>
+      </c>
+      <c r="C841" t="s">
+        <v>465</v>
+      </c>
+      <c r="D841">
+        <v>3</v>
+      </c>
+      <c r="E841" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="842" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A842" s="1">
+        <v>44712</v>
+      </c>
+      <c r="B842" t="s">
+        <v>349</v>
+      </c>
+      <c r="C842" t="s">
+        <v>349</v>
+      </c>
+      <c r="D842">
+        <v>4</v>
+      </c>
+      <c r="E842" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="843" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A843" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B843" t="s">
+        <v>466</v>
+      </c>
+      <c r="C843" t="s">
+        <v>8</v>
+      </c>
+      <c r="D843">
+        <v>1</v>
+      </c>
+      <c r="E843" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="844" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A844" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B844" t="s">
+        <v>466</v>
+      </c>
+      <c r="C844" t="s">
+        <v>467</v>
+      </c>
+      <c r="D844">
+        <v>2</v>
+      </c>
+      <c r="E844" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="845" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A845" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B845" t="s">
+        <v>466</v>
+      </c>
+      <c r="C845" t="s">
+        <v>466</v>
+      </c>
+      <c r="D845">
+        <v>3</v>
+      </c>
+      <c r="E845" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="846" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A846" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B846" t="s">
+        <v>466</v>
+      </c>
+      <c r="C846" t="s">
+        <v>13</v>
+      </c>
+      <c r="D846">
+        <v>1</v>
+      </c>
+      <c r="E846" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="847" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A847" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B847" t="s">
+        <v>466</v>
+      </c>
+      <c r="C847" t="s">
+        <v>467</v>
+      </c>
+      <c r="D847">
+        <v>2</v>
+      </c>
+      <c r="E847" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="848" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A848" s="1">
+        <v>44713</v>
+      </c>
+      <c r="B848" t="s">
+        <v>466</v>
+      </c>
+      <c r="C848" t="s">
+        <v>466</v>
+      </c>
+      <c r="D848">
+        <v>3</v>
+      </c>
+      <c r="E848" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="849" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A849" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B849" t="s">
+        <v>468</v>
+      </c>
+      <c r="C849" t="s">
+        <v>8</v>
+      </c>
+      <c r="D849">
+        <v>1</v>
+      </c>
+      <c r="E849" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="850" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A850" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B850" t="s">
+        <v>468</v>
+      </c>
+      <c r="C850" t="s">
+        <v>30</v>
+      </c>
+      <c r="D850">
+        <v>2</v>
+      </c>
+      <c r="E850" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="851" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A851" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B851" t="s">
+        <v>468</v>
+      </c>
+      <c r="C851" t="s">
+        <v>318</v>
+      </c>
+      <c r="D851">
+        <v>3</v>
+      </c>
+      <c r="E851" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="852" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A852" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B852" t="s">
+        <v>468</v>
+      </c>
+      <c r="C852" t="s">
+        <v>469</v>
+      </c>
+      <c r="D852">
+        <v>4</v>
+      </c>
+      <c r="E852" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="853" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A853" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B853" t="s">
+        <v>468</v>
+      </c>
+      <c r="C853" t="s">
+        <v>468</v>
+      </c>
+      <c r="D853">
+        <v>5</v>
+      </c>
+      <c r="E853" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="854" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A854" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B854" t="s">
+        <v>468</v>
+      </c>
+      <c r="C854" t="s">
+        <v>13</v>
+      </c>
+      <c r="D854">
+        <v>1</v>
+      </c>
+      <c r="E854" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="855" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A855" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B855" t="s">
+        <v>468</v>
+      </c>
+      <c r="C855" t="s">
+        <v>29</v>
+      </c>
+      <c r="D855">
+        <v>2</v>
+      </c>
+      <c r="E855" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="856" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A856" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B856" t="s">
+        <v>468</v>
+      </c>
+      <c r="C856" t="s">
+        <v>469</v>
+      </c>
+      <c r="D856">
+        <v>3</v>
+      </c>
+      <c r="E856" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="857" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A857" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B857" t="s">
+        <v>468</v>
+      </c>
+      <c r="C857" t="s">
+        <v>318</v>
+      </c>
+      <c r="D857">
+        <v>4</v>
+      </c>
+      <c r="E857" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="858" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A858" s="1">
+        <v>44714</v>
+      </c>
+      <c r="B858" t="s">
+        <v>468</v>
+      </c>
+      <c r="C858" t="s">
+        <v>468</v>
+      </c>
+      <c r="D858">
+        <v>5</v>
+      </c>
+      <c r="E858" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="859" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A859" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B859" t="s">
+        <v>471</v>
+      </c>
+      <c r="C859" t="s">
+        <v>8</v>
+      </c>
+      <c r="D859">
+        <v>1</v>
+      </c>
+      <c r="E859" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="860" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A860" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B860" t="s">
+        <v>471</v>
+      </c>
+      <c r="C860" t="s">
+        <v>470</v>
+      </c>
+      <c r="D860">
+        <v>2</v>
+      </c>
+      <c r="E860" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="861" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A861" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B861" t="s">
+        <v>471</v>
+      </c>
+      <c r="C861" t="s">
+        <v>471</v>
+      </c>
+      <c r="D861">
+        <v>3</v>
+      </c>
+      <c r="E861" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="862" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A862" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B862" t="s">
+        <v>471</v>
+      </c>
+      <c r="C862" t="s">
+        <v>13</v>
+      </c>
+      <c r="D862">
+        <v>1</v>
+      </c>
+      <c r="E862" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="863" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A863" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B863" t="s">
+        <v>471</v>
+      </c>
+      <c r="C863" t="s">
+        <v>274</v>
+      </c>
+      <c r="D863">
+        <v>2</v>
+      </c>
+      <c r="E863" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="864" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A864" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B864" t="s">
+        <v>471</v>
+      </c>
+      <c r="C864" t="s">
+        <v>472</v>
+      </c>
+      <c r="D864">
+        <v>3</v>
+      </c>
+      <c r="E864" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="865" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A865" s="1">
+        <v>44715</v>
+      </c>
+      <c r="B865" t="s">
+        <v>471</v>
+      </c>
+      <c r="C865" t="s">
+        <v>471</v>
+      </c>
+      <c r="D865">
+        <v>4</v>
+      </c>
+      <c r="E865" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="866" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A866" s="1">
+        <v>44716</v>
+      </c>
+      <c r="B866" t="s">
+        <v>473</v>
+      </c>
+      <c r="C866" t="s">
+        <v>8</v>
+      </c>
+      <c r="D866">
+        <v>1</v>
+      </c>
+      <c r="E866" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="867" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A867" s="1">
+        <v>44716</v>
+      </c>
+      <c r="B867" t="s">
+        <v>473</v>
+      </c>
+      <c r="C867" t="s">
+        <v>473</v>
+      </c>
+      <c r="D867">
+        <v>2</v>
+      </c>
+      <c r="E867" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="868" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A868" s="1">
+        <v>44717</v>
+      </c>
+      <c r="B868" t="s">
+        <v>474</v>
+      </c>
+      <c r="C868" t="s">
+        <v>8</v>
+      </c>
+      <c r="D868">
+        <v>1</v>
+      </c>
+      <c r="E868" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="869" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A869" s="1">
+        <v>44717</v>
+      </c>
+      <c r="B869" t="s">
+        <v>474</v>
+      </c>
+      <c r="C869" t="s">
+        <v>475</v>
+      </c>
+      <c r="D869">
+        <v>2</v>
+      </c>
+      <c r="E869" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="870" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A870" s="1">
+        <v>44717</v>
+      </c>
+      <c r="B870" t="s">
+        <v>474</v>
+      </c>
+      <c r="C870" t="s">
+        <v>474</v>
+      </c>
+      <c r="D870">
+        <v>3</v>
+      </c>
+      <c r="E870" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="871" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A871" s="1">
+        <v>44717</v>
+      </c>
+      <c r="B871" t="s">
+        <v>474</v>
+      </c>
+      <c r="C871" t="s">
+        <v>13</v>
+      </c>
+      <c r="D871">
+        <v>1</v>
+      </c>
+      <c r="E871" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="872" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A872" s="1">
+        <v>44717</v>
+      </c>
+      <c r="B872" t="s">
+        <v>474</v>
+      </c>
+      <c r="C872" t="s">
+        <v>476</v>
+      </c>
+      <c r="D872">
+        <v>2</v>
+      </c>
+      <c r="E872" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="873" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A873" s="1">
+        <v>44717</v>
+      </c>
+      <c r="B873" t="s">
+        <v>474</v>
+      </c>
+      <c r="C873" t="s">
+        <v>477</v>
+      </c>
+      <c r="D873">
+        <v>3</v>
+      </c>
+      <c r="E873" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="874" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A874" s="1">
+        <v>44717</v>
+      </c>
+      <c r="B874" t="s">
+        <v>474</v>
+      </c>
+      <c r="C874" t="s">
+        <v>474</v>
+      </c>
+      <c r="D874">
+        <v>4</v>
+      </c>
+      <c r="E874" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="875" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A875" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B875" t="s">
+        <v>478</v>
+      </c>
+      <c r="C875" t="s">
+        <v>8</v>
+      </c>
+      <c r="D875">
+        <v>1</v>
+      </c>
+      <c r="E875" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="876" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A876" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B876" t="s">
+        <v>478</v>
+      </c>
+      <c r="C876" t="s">
+        <v>479</v>
+      </c>
+      <c r="D876">
+        <v>2</v>
+      </c>
+      <c r="E876" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="877" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A877" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B877" t="s">
+        <v>478</v>
+      </c>
+      <c r="C877" t="s">
+        <v>480</v>
+      </c>
+      <c r="D877">
+        <v>3</v>
+      </c>
+      <c r="E877" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="878" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A878" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B878" t="s">
+        <v>478</v>
+      </c>
+      <c r="C878" t="s">
+        <v>481</v>
+      </c>
+      <c r="D878">
+        <v>4</v>
+      </c>
+      <c r="E878" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="879" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A879" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B879" t="s">
+        <v>478</v>
+      </c>
+      <c r="C879" t="s">
+        <v>478</v>
+      </c>
+      <c r="D879">
+        <v>5</v>
+      </c>
+      <c r="E879" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="880" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A880" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B880" t="s">
+        <v>478</v>
+      </c>
+      <c r="C880" t="s">
+        <v>13</v>
+      </c>
+      <c r="D880">
+        <v>1</v>
+      </c>
+      <c r="E880" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="881" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A881" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B881" t="s">
+        <v>478</v>
+      </c>
+      <c r="C881" t="s">
+        <v>29</v>
+      </c>
+      <c r="D881">
+        <v>2</v>
+      </c>
+      <c r="E881" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="882" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A882" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B882" t="s">
+        <v>478</v>
+      </c>
+      <c r="C882" t="s">
+        <v>482</v>
+      </c>
+      <c r="D882">
+        <v>3</v>
+      </c>
+      <c r="E882" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="883" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A883" s="1">
+        <v>44718</v>
+      </c>
+      <c r="B883" t="s">
+        <v>478</v>
+      </c>
+      <c r="C883" t="s">
+        <v>478</v>
+      </c>
+      <c r="D883">
+        <v>4</v>
+      </c>
+      <c r="E883" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="884" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A884" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B884" t="s">
+        <v>483</v>
+      </c>
+      <c r="C884" t="s">
+        <v>8</v>
+      </c>
+      <c r="D884">
+        <v>1</v>
+      </c>
+      <c r="E884" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="885" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A885" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B885" t="s">
+        <v>483</v>
+      </c>
+      <c r="C885" t="s">
+        <v>30</v>
+      </c>
+      <c r="D885">
+        <v>2</v>
+      </c>
+      <c r="E885" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="886" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A886" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B886" t="s">
+        <v>483</v>
+      </c>
+      <c r="C886" t="s">
+        <v>484</v>
+      </c>
+      <c r="D886">
+        <v>3</v>
+      </c>
+      <c r="E886" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="887" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A887" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B887" t="s">
+        <v>483</v>
+      </c>
+      <c r="C887" t="s">
+        <v>485</v>
+      </c>
+      <c r="D887">
+        <v>4</v>
+      </c>
+      <c r="E887" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="888" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A888" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B888" t="s">
+        <v>483</v>
+      </c>
+      <c r="C888" t="s">
+        <v>483</v>
+      </c>
+      <c r="D888">
+        <v>5</v>
+      </c>
+      <c r="E888" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="889" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A889" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B889" t="s">
+        <v>483</v>
+      </c>
+      <c r="C889" t="s">
+        <v>13</v>
+      </c>
+      <c r="D889">
+        <v>1</v>
+      </c>
+      <c r="E889" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="890" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A890" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B890" t="s">
+        <v>483</v>
+      </c>
+      <c r="C890" t="s">
+        <v>194</v>
+      </c>
+      <c r="D890">
+        <v>2</v>
+      </c>
+      <c r="E890" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="891" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A891" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B891" t="s">
+        <v>483</v>
+      </c>
+      <c r="C891" t="s">
+        <v>483</v>
+      </c>
+      <c r="D891">
+        <v>3</v>
+      </c>
+      <c r="E891" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="892" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A892" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B892" t="s">
+        <v>486</v>
+      </c>
+      <c r="C892" t="s">
+        <v>8</v>
+      </c>
+      <c r="D892">
+        <v>1</v>
+      </c>
+      <c r="E892" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="893" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A893" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B893" t="s">
+        <v>486</v>
+      </c>
+      <c r="C893" t="s">
+        <v>487</v>
+      </c>
+      <c r="D893">
+        <v>2</v>
+      </c>
+      <c r="E893" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="894" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A894" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B894" t="s">
+        <v>486</v>
+      </c>
+      <c r="C894" t="s">
+        <v>326</v>
+      </c>
+      <c r="D894">
+        <v>3</v>
+      </c>
+      <c r="E894" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="895" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A895" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B895" t="s">
+        <v>486</v>
+      </c>
+      <c r="C895" t="s">
+        <v>486</v>
+      </c>
+      <c r="D895">
+        <v>4</v>
+      </c>
+      <c r="E895" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="896" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A896" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B896" t="s">
+        <v>486</v>
+      </c>
+      <c r="C896" t="s">
+        <v>13</v>
+      </c>
+      <c r="D896">
+        <v>1</v>
+      </c>
+      <c r="E896" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="897" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A897" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B897" t="s">
+        <v>486</v>
+      </c>
+      <c r="C897" t="s">
+        <v>488</v>
+      </c>
+      <c r="D897">
+        <v>2</v>
+      </c>
+      <c r="E897" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="898" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A898" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B898" t="s">
+        <v>486</v>
+      </c>
+      <c r="C898" t="s">
+        <v>489</v>
+      </c>
+      <c r="D898">
+        <v>3</v>
+      </c>
+      <c r="E898" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="899" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A899" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B899" t="s">
+        <v>486</v>
+      </c>
+      <c r="C899" t="s">
+        <v>358</v>
+      </c>
+      <c r="D899">
+        <v>4</v>
+      </c>
+      <c r="E899" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="900" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A900" s="1">
+        <v>44720</v>
+      </c>
+      <c r="B900" t="s">
+        <v>486</v>
+      </c>
+      <c r="C900" t="s">
+        <v>486</v>
+      </c>
+      <c r="D900">
+        <v>5</v>
+      </c>
+      <c r="E900" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="901" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A901" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B901" t="s">
+        <v>490</v>
+      </c>
+      <c r="C901" t="s">
+        <v>8</v>
+      </c>
+      <c r="D901">
+        <v>1</v>
+      </c>
+      <c r="E901" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="902" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A902" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B902" t="s">
+        <v>490</v>
+      </c>
+      <c r="C902" t="s">
+        <v>345</v>
+      </c>
+      <c r="D902">
+        <v>2</v>
+      </c>
+      <c r="E902" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="903" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A903" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B903" t="s">
+        <v>490</v>
+      </c>
+      <c r="C903" t="s">
+        <v>490</v>
+      </c>
+      <c r="D903">
+        <v>3</v>
+      </c>
+      <c r="E903" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="904" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A904" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B904" t="s">
+        <v>490</v>
+      </c>
+      <c r="C904" t="s">
+        <v>13</v>
+      </c>
+      <c r="D904">
+        <v>1</v>
+      </c>
+      <c r="E904" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="905" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A905" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B905" t="s">
+        <v>490</v>
+      </c>
+      <c r="C905" t="s">
+        <v>491</v>
+      </c>
+      <c r="D905">
+        <v>2</v>
+      </c>
+      <c r="E905" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="906" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A906" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B906" t="s">
+        <v>490</v>
+      </c>
+      <c r="C906" t="s">
+        <v>492</v>
+      </c>
+      <c r="D906">
+        <v>3</v>
+      </c>
+      <c r="E906" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="907" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A907" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B907" t="s">
+        <v>490</v>
+      </c>
+      <c r="C907" t="s">
+        <v>493</v>
+      </c>
+      <c r="D907">
+        <v>4</v>
+      </c>
+      <c r="E907" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="908" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A908" s="1">
+        <v>44721</v>
+      </c>
+      <c r="B908" t="s">
+        <v>490</v>
+      </c>
+      <c r="C908" t="s">
+        <v>490</v>
+      </c>
+      <c r="D908">
+        <v>5</v>
+      </c>
+      <c r="E908" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="909" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A909" s="1">
+        <v>44722</v>
+      </c>
+      <c r="B909" t="s">
+        <v>497</v>
+      </c>
+      <c r="C909" t="s">
+        <v>13</v>
+      </c>
+      <c r="D909">
+        <v>1</v>
+      </c>
+      <c r="E909" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="910" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A910" s="1">
+        <v>44722</v>
+      </c>
+      <c r="B910" t="s">
+        <v>497</v>
+      </c>
+      <c r="C910" t="s">
+        <v>107</v>
+      </c>
+      <c r="D910">
+        <v>2</v>
+      </c>
+      <c r="E910" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="911" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A911" s="1">
+        <v>44722</v>
+      </c>
+      <c r="B911" t="s">
+        <v>497</v>
+      </c>
+      <c r="C911" t="s">
+        <v>496</v>
+      </c>
+      <c r="D911">
+        <v>3</v>
+      </c>
+      <c r="E911" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="912" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A912" s="1">
+        <v>44722</v>
+      </c>
+      <c r="B912" t="s">
+        <v>497</v>
+      </c>
+      <c r="C912" t="s">
+        <v>475</v>
+      </c>
+      <c r="D912">
+        <v>4</v>
+      </c>
+      <c r="E912" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="913" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A913" s="1">
+        <v>44722</v>
+      </c>
+      <c r="B913" t="s">
+        <v>497</v>
+      </c>
+      <c r="C913" t="s">
+        <v>497</v>
+      </c>
+      <c r="D913">
+        <v>5</v>
+      </c>
+      <c r="E913" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="914" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A914" s="1">
+        <v>44723</v>
+      </c>
+      <c r="B914" t="s">
+        <v>494</v>
+      </c>
+      <c r="C914" t="s">
+        <v>8</v>
+      </c>
+      <c r="D914">
+        <v>1</v>
+      </c>
+      <c r="E914" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="915" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A915" s="1">
+        <v>44723</v>
+      </c>
+      <c r="B915" t="s">
+        <v>494</v>
+      </c>
+      <c r="C915" t="s">
+        <v>152</v>
+      </c>
+      <c r="D915">
+        <v>2</v>
+      </c>
+      <c r="E915" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="916" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A916" s="1">
+        <v>44723</v>
+      </c>
+      <c r="B916" t="s">
+        <v>494</v>
+      </c>
+      <c r="C916" t="s">
+        <v>495</v>
+      </c>
+      <c r="D916">
+        <v>3</v>
+      </c>
+      <c r="E916" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="917" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A917" s="1">
+        <v>44723</v>
+      </c>
+      <c r="B917" t="s">
+        <v>494</v>
+      </c>
+      <c r="C917" t="s">
+        <v>494</v>
+      </c>
+      <c r="D917">
+        <v>4</v>
+      </c>
+      <c r="E917" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="918" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A918" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B918" t="s">
+        <v>498</v>
+      </c>
+      <c r="C918" t="s">
+        <v>8</v>
+      </c>
+      <c r="D918">
+        <v>1</v>
+      </c>
+      <c r="E918" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="919" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A919" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B919" t="s">
+        <v>498</v>
+      </c>
+      <c r="C919" t="s">
+        <v>499</v>
+      </c>
+      <c r="D919">
+        <v>2</v>
+      </c>
+      <c r="E919" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="920" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A920" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B920" t="s">
+        <v>498</v>
+      </c>
+      <c r="C920" t="s">
+        <v>77</v>
+      </c>
+      <c r="D920">
+        <v>3</v>
+      </c>
+      <c r="E920" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="921" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A921" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B921" t="s">
+        <v>498</v>
+      </c>
+      <c r="C921" t="s">
+        <v>498</v>
+      </c>
+      <c r="D921">
+        <v>4</v>
+      </c>
+      <c r="E921" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="922" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A922" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B922" t="s">
+        <v>498</v>
+      </c>
+      <c r="C922" t="s">
+        <v>13</v>
+      </c>
+      <c r="D922">
+        <v>1</v>
+      </c>
+      <c r="E922" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="923" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A923" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B923" t="s">
+        <v>498</v>
+      </c>
+      <c r="C923" t="s">
+        <v>500</v>
+      </c>
+      <c r="D923">
+        <v>2</v>
+      </c>
+      <c r="E923" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="924" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A924" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B924" t="s">
+        <v>498</v>
+      </c>
+      <c r="C924" t="s">
+        <v>501</v>
+      </c>
+      <c r="D924">
+        <v>3</v>
+      </c>
+      <c r="E924" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="925" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A925" s="1">
+        <v>44725</v>
+      </c>
+      <c r="B925" t="s">
+        <v>498</v>
+      </c>
+      <c r="C925" t="s">
+        <v>498</v>
+      </c>
+      <c r="D925">
+        <v>4</v>
+      </c>
+      <c r="E925" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="926" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A926" s="1">
+        <v>44726</v>
+      </c>
+      <c r="B926" t="s">
+        <v>503</v>
+      </c>
+      <c r="C926" t="s">
+        <v>8</v>
+      </c>
+      <c r="D926">
+        <v>1</v>
+      </c>
+      <c r="E926" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="927" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A927" s="1">
+        <v>44726</v>
+      </c>
+      <c r="B927" t="s">
+        <v>503</v>
+      </c>
+      <c r="C927" t="s">
+        <v>502</v>
+      </c>
+      <c r="D927">
+        <v>2</v>
+      </c>
+      <c r="E927" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="928" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A928" s="1">
+        <v>44726</v>
+      </c>
+      <c r="B928" t="s">
+        <v>503</v>
+      </c>
+      <c r="C928" t="s">
+        <v>503</v>
+      </c>
+      <c r="D928">
+        <v>3</v>
+      </c>
+      <c r="E928" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="929" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A929" s="1">
+        <v>44727</v>
+      </c>
+      <c r="B929" t="s">
+        <v>504</v>
+      </c>
+      <c r="C929" t="s">
+        <v>8</v>
+      </c>
+      <c r="D929">
+        <v>1</v>
+      </c>
+      <c r="E929" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="930" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A930" s="1">
+        <v>44727</v>
+      </c>
+      <c r="B930" t="s">
+        <v>504</v>
+      </c>
+      <c r="C930" t="s">
+        <v>505</v>
+      </c>
+      <c r="D930">
+        <v>2</v>
+      </c>
+      <c r="E930" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="931" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A931" s="1">
+        <v>44727</v>
+      </c>
+      <c r="B931" t="s">
+        <v>504</v>
+      </c>
+      <c r="C931" t="s">
+        <v>506</v>
+      </c>
+      <c r="D931">
+        <v>3</v>
+      </c>
+      <c r="E931" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="932" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A932" s="1">
+        <v>44727</v>
+      </c>
+      <c r="B932" t="s">
+        <v>504</v>
+      </c>
+      <c r="C932" t="s">
+        <v>504</v>
+      </c>
+      <c r="D932">
+        <v>4</v>
+      </c>
+      <c r="E932" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="933" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A933" s="1">
+        <v>44727</v>
+      </c>
+      <c r="B933" t="s">
+        <v>504</v>
+      </c>
+      <c r="C933" t="s">
+        <v>13</v>
+      </c>
+      <c r="D933">
+        <v>1</v>
+      </c>
+      <c r="E933" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="934" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A934" s="1">
+        <v>44727</v>
+      </c>
+      <c r="B934" t="s">
+        <v>504</v>
+      </c>
+      <c r="C934" t="s">
+        <v>45</v>
+      </c>
+      <c r="D934">
+        <v>2</v>
+      </c>
+      <c r="E934" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="935" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A935" s="1">
+        <v>44727</v>
+      </c>
+      <c r="B935" t="s">
+        <v>504</v>
+      </c>
+      <c r="C935" t="s">
+        <v>504</v>
+      </c>
+      <c r="D935">
+        <v>3</v>
+      </c>
+      <c r="E935" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="936" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A936" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B936" t="s">
+        <v>507</v>
+      </c>
+      <c r="C936" t="s">
+        <v>8</v>
+      </c>
+      <c r="D936">
+        <v>1</v>
+      </c>
+      <c r="E936" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="937" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A937" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B937" t="s">
+        <v>507</v>
+      </c>
+      <c r="C937" t="s">
+        <v>463</v>
+      </c>
+      <c r="D937">
+        <v>2</v>
+      </c>
+      <c r="E937" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="938" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A938" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B938" t="s">
+        <v>507</v>
+      </c>
+      <c r="C938" t="s">
+        <v>507</v>
+      </c>
+      <c r="D938">
+        <v>3</v>
+      </c>
+      <c r="E938" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="939" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A939" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B939" t="s">
+        <v>507</v>
+      </c>
+      <c r="C939" t="s">
+        <v>13</v>
+      </c>
+      <c r="D939">
+        <v>1</v>
+      </c>
+      <c r="E939" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="940" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A940" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B940" t="s">
+        <v>507</v>
+      </c>
+      <c r="C940" t="s">
+        <v>508</v>
+      </c>
+      <c r="D940">
+        <v>2</v>
+      </c>
+      <c r="E940" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="941" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A941" s="1">
+        <v>44728</v>
+      </c>
+      <c r="B941" t="s">
+        <v>507</v>
+      </c>
+      <c r="C941" t="s">
+        <v>507</v>
+      </c>
+      <c r="D941">
+        <v>3</v>
+      </c>
+      <c r="E941" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>